<commit_message>
Running User login and logut scenarios
</commit_message>
<xml_diff>
--- a/src/test/resources/UserDataFile.xlsx
+++ b/src/test/resources/UserDataFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="10560"/>
+    <workbookView windowWidth="28800" windowHeight="10560" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LoginSheet" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="86">
   <si>
     <t>Scenario</t>
   </si>
@@ -283,10 +283,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -359,16 +359,24 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -381,22 +389,7 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -411,6 +404,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -428,14 +428,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -450,7 +465,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -464,25 +479,10 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -513,31 +513,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -549,55 +669,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -609,89 +681,41 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -719,15 +743,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -739,21 +754,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -792,149 +792,164 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -942,19 +957,31 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="48">
       <alignment vertical="center"/>
     </xf>
@@ -962,6 +989,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="48" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -1324,8 +1354,8 @@
   <sheetPr/>
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="7"/>
@@ -1339,55 +1369,55 @@
     <col min="8" max="8" width="14.5625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="1" ht="15.2" spans="1:8">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="11" customFormat="1" ht="15.2" spans="1:8">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" s="3" customFormat="1" ht="15" spans="1:8">
-      <c r="A2" s="9" t="s">
+    <row r="2" s="6" customFormat="1" ht="15" spans="1:8">
+      <c r="A2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="6">
         <v>200</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1395,19 +1425,19 @@
       <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="6" t="s">
         <v>13</v>
       </c>
       <c r="G3">
@@ -1424,13 +1454,13 @@
       <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="18" t="s">
         <v>19</v>
       </c>
       <c r="G4">
@@ -1441,19 +1471,19 @@
       <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="6" t="s">
         <v>13</v>
       </c>
       <c r="G5">
@@ -1464,19 +1494,19 @@
       <c r="A6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="6" t="s">
         <v>13</v>
       </c>
       <c r="G6">
@@ -1487,22 +1517,22 @@
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="6">
         <v>200</v>
       </c>
       <c r="H7" t="s">
@@ -1513,19 +1543,19 @@
       <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C8" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="6" t="s">
         <v>13</v>
       </c>
       <c r="G8">
@@ -1536,19 +1566,19 @@
       <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="8" t="s">
         <v>29</v>
       </c>
       <c r="C9" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="18" t="s">
         <v>19</v>
       </c>
       <c r="G9">
@@ -1559,19 +1589,19 @@
       <c r="A10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="6" t="s">
         <v>13</v>
       </c>
       <c r="G10">
@@ -1582,19 +1612,19 @@
       <c r="A11" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="6" t="s">
         <v>13</v>
       </c>
       <c r="G11">
@@ -1605,22 +1635,22 @@
       <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="6">
         <v>200</v>
       </c>
       <c r="H12" t="s">
@@ -1637,13 +1667,13 @@
       <c r="C13" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="6" t="s">
         <v>13</v>
       </c>
       <c r="G13">
@@ -1654,19 +1684,19 @@
       <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="8" t="s">
         <v>34</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="18" t="s">
         <v>19</v>
       </c>
       <c r="G14">
@@ -1677,19 +1707,19 @@
       <c r="A15" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="8" t="s">
         <v>34</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="6" t="s">
         <v>13</v>
       </c>
       <c r="G15">
@@ -1700,19 +1730,19 @@
       <c r="A16" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="8" t="s">
         <v>34</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="6" t="s">
         <v>13</v>
       </c>
       <c r="G16">
@@ -1744,7 +1774,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A2" sqref="$A2:$XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2"/>
@@ -1803,13 +1833,13 @@
       <c r="B2">
         <v>7686123101</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="23" t="s">
         <v>47</v>
       </c>
       <c r="D2" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="10" t="s">
         <v>49</v>
       </c>
       <c r="F2" t="s">
@@ -1838,13 +1868,13 @@
       <c r="B3">
         <v>7686123102</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="23" t="s">
         <v>56</v>
       </c>
       <c r="D3" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="8" t="s">
         <v>58</v>
       </c>
       <c r="F3" t="s">
@@ -1939,7 +1969,7 @@
       <c r="D2">
         <v>6375480001</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="8" t="s">
         <v>72</v>
       </c>
       <c r="F2" t="s">
@@ -1951,7 +1981,7 @@
       <c r="H2" t="s">
         <v>75</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="24" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1968,7 +1998,7 @@
       <c r="D3">
         <v>6375480002</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="8" t="s">
         <v>80</v>
       </c>
       <c r="F3" t="s">
@@ -1980,7 +2010,7 @@
       <c r="H3" t="s">
         <v>75</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="24" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1997,117 +2027,224 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D$1:D$1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="6" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="13.4375" customWidth="1"/>
     <col min="2" max="2" width="18.5" customWidth="1"/>
     <col min="3" max="3" width="13.4375" customWidth="1"/>
-    <col min="4" max="4" width="14.5625" customWidth="1"/>
+    <col min="5" max="5" width="14.5625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.8" spans="1:4">
-      <c r="A1" t="s">
+    <row r="1" ht="14.8" spans="1:5">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>200</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>200</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>200</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="1">
+        <v>400</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C5">
+      <c r="C6" s="1">
         <v>404</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C6">
+      <c r="C7" s="1">
         <v>404</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C7">
+      <c r="C8" s="1">
         <v>404</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>32</v>
       </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="1">
+        <v>405</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="1">
+        <v>405</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="1">
+        <v>405</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="4:4">
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="4:4">
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="4:4">
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="4:4">
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="4:4">
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="4:4">
+      <c r="D17" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>